<commit_message>
add webhook url to main app
</commit_message>
<xml_diff>
--- a/file_manager/rental_order.xlsx
+++ b/file_manager/rental_order.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiquethomas/Documents/GitHub/File-Manager/file_manager/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikthomas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014637B5-0824-304B-BEA0-DF65D9AA0BBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CB8A8E-3E37-0749-8D20-8D270A033853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23820" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,38 +19,38 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="bBuyerAddress">[1]Settings!$G$7="ON"</definedName>
-    <definedName name="bBuyerCity">[1]Settings!$G$8="ON"</definedName>
-    <definedName name="bBuyerFax">[1]Settings!$G$10="ON"</definedName>
-    <definedName name="bBuyerName">[1]Settings!$G$6="ON"</definedName>
-    <definedName name="bBuyerPhone">[1]Settings!$G$9="ON"</definedName>
-    <definedName name="bFOBIncoterm">[1]Settings!$G$20="ON"</definedName>
-    <definedName name="bNumPackages">[1]Settings!$G$21="ON"</definedName>
-    <definedName name="bPONumber">[1]Settings!$G$16="ON"</definedName>
-    <definedName name="bSalesperson">[1]Settings!$G$17="ON"</definedName>
-    <definedName name="bSellerAddress">[1]Settings!$G$12="ON"</definedName>
-    <definedName name="bSellerCity">[1]Settings!$G$13="ON"</definedName>
-    <definedName name="bSellerFax">[1]Settings!$G$15="ON"</definedName>
-    <definedName name="bSellerName">[1]Settings!$G$11="ON"</definedName>
-    <definedName name="bSellerPhone">[1]Settings!$G$14="ON"</definedName>
-    <definedName name="bShippedVia">[1]Settings!$G$18="ON"</definedName>
-    <definedName name="bTerms">[1]Settings!$G$19="ON"</definedName>
-    <definedName name="BuyerAddress">[1]Invoice!$G$6</definedName>
-    <definedName name="BuyerCityStateZip">[1]Invoice!$G$7</definedName>
-    <definedName name="BuyerFax">[1]Invoice!$G$9</definedName>
-    <definedName name="BuyerName">[1]Invoice!$G$5</definedName>
-    <definedName name="BuyerPhone">[1]Invoice!$G$8</definedName>
-    <definedName name="invFOBIncoterm">[1]Invoice!$F$16</definedName>
-    <definedName name="invNumPackages">[1]Invoice!$K$13</definedName>
-    <definedName name="invPONumber">[1]Invoice!$F$13</definedName>
-    <definedName name="invSalesperson">[1]Invoice!$B$13</definedName>
-    <definedName name="invShippedVia">[1]Invoice!$M$13</definedName>
-    <definedName name="invTerms">[1]Invoice!$B$16</definedName>
-    <definedName name="SellerAddress">[1]Invoice!$B$6</definedName>
-    <definedName name="SellerCityStateZip">[1]Invoice!$B$7</definedName>
-    <definedName name="SellerFax">[1]Invoice!$B$9</definedName>
-    <definedName name="SellerName">[1]Invoice!$B$5</definedName>
-    <definedName name="SellerPhone">[1]Invoice!$B$8</definedName>
+    <definedName name="bBuyerAddress">[1]Sheet1!$G$7="ON"</definedName>
+    <definedName name="bBuyerCity">[1]Sheet1!$G$8="ON"</definedName>
+    <definedName name="bBuyerFax">[1]Sheet1!$G$10="ON"</definedName>
+    <definedName name="bBuyerName">[1]Sheet1!$G$6="ON"</definedName>
+    <definedName name="bBuyerPhone">[1]Sheet1!$G$9="ON"</definedName>
+    <definedName name="bFOBIncoterm">[1]Sheet1!$G$20="ON"</definedName>
+    <definedName name="bNumPackages">[1]Sheet1!$G$21="ON"</definedName>
+    <definedName name="bPONumber">[1]Sheet1!$G$16="ON"</definedName>
+    <definedName name="bSalesperson">[1]Sheet1!$G$17="ON"</definedName>
+    <definedName name="bSellerAddress">[1]Sheet1!$G$12="ON"</definedName>
+    <definedName name="bSellerCity">[1]Sheet1!$G$13="ON"</definedName>
+    <definedName name="bSellerFax">[1]Sheet1!$G$15="ON"</definedName>
+    <definedName name="bSellerName">[1]Sheet1!$G$11="ON"</definedName>
+    <definedName name="bSellerPhone">[1]Sheet1!$G$14="ON"</definedName>
+    <definedName name="bShippedVia">[1]Sheet1!$G$18="ON"</definedName>
+    <definedName name="bTerms">[1]Sheet1!$G$19="ON"</definedName>
+    <definedName name="BuyerAddress">[1]Sheet1!$G$6</definedName>
+    <definedName name="BuyerCityStateZip">[1]Sheet1!$G$7</definedName>
+    <definedName name="BuyerFax">[1]Sheet1!$G$9</definedName>
+    <definedName name="BuyerName">[1]Sheet1!$G$5</definedName>
+    <definedName name="BuyerPhone">[1]Sheet1!$G$8</definedName>
+    <definedName name="invFOBIncoterm">[1]Sheet1!$F$16</definedName>
+    <definedName name="invNumPackages">[1]Sheet1!$K$13</definedName>
+    <definedName name="invPONumber">[1]Sheet1!$F$13</definedName>
+    <definedName name="invSalesperson">[1]Sheet1!$B$13</definedName>
+    <definedName name="invShippedVia">[1]Sheet1!$M$13</definedName>
+    <definedName name="invTerms">[1]Sheet1!$B$16</definedName>
+    <definedName name="SellerAddress">[1]Sheet1!$B$6</definedName>
+    <definedName name="SellerCityStateZip">[1]Sheet1!$B$7</definedName>
+    <definedName name="SellerFax">[1]Sheet1!$B$9</definedName>
+    <definedName name="SellerName">[1]Sheet1!$B$5</definedName>
+    <definedName name="SellerPhone">[1]Sheet1!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -68,15 +68,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>TAGGABOX</t>
   </si>
   <si>
     <t>Rental Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INVOICE: </t>
   </si>
   <si>
     <t>503 Commerce Park DR SE</t>
@@ -195,7 +192,7 @@
     <numFmt numFmtId="165" formatCode="@\ \ "/>
     <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,13 +228,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -264,15 +254,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="28"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -281,12 +285,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -300,6 +298,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -449,15 +453,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FFC00000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="dotted">
         <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
@@ -553,12 +548,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -579,135 +583,144 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1067,156 +1080,49 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Sheet1"/>
       <sheetName val="Invoice"/>
-      <sheetName val="Settings"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="5">
-          <cell r="B5" t="str">
-            <v>Contoso, Ltd</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>Graphic Design Institute</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>567 First Street</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>2345 Main Street</v>
-          </cell>
+          <cell r="B5"/>
+          <cell r="G5"/>
         </row>
         <row r="7">
           <cell r="B7" t="str">
-            <v>Cherryville, WA 12345</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>Gateway, OH 12345</v>
+            <v>BUYER</v>
           </cell>
         </row>
-        <row r="8">
-          <cell r="B8">
-            <v>8885550104</v>
-          </cell>
-          <cell r="G8">
-            <v>5095550192</v>
-          </cell>
+        <row r="14">
+          <cell r="G14"/>
         </row>
-        <row r="9">
-          <cell r="B9">
-            <v>8885550105</v>
-          </cell>
-          <cell r="G9">
-            <v>5095550193</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Kim Abercrombie</v>
-          </cell>
-          <cell r="F13">
-            <v>123</v>
-          </cell>
-          <cell r="K13">
-            <v>1</v>
-          </cell>
-          <cell r="M13" t="str">
-            <v>USPS</v>
+        <row r="15">
+          <cell r="G15" t="str">
+            <v>PICK UP</v>
           </cell>
         </row>
         <row r="16">
-          <cell r="B16" t="str">
-            <v>None</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>Freight prepaid</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="6">
-          <cell r="G6" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="G7" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="G8" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="G9" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10" t="str">
-            <v>OFF</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="G11" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="G12" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="G13" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="G14" t="str">
-            <v>ON</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="G15" t="str">
-            <v>OFF</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="G16" t="str">
-            <v>ON</v>
-          </cell>
+          <cell r="B16"/>
+          <cell r="F16"/>
+          <cell r="G16"/>
         </row>
         <row r="17">
           <cell r="G17" t="str">
-            <v>ON</v>
+            <v>SHIPPED</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="G18" t="str">
-            <v>OFF</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="G19" t="str">
-            <v>OFF</v>
-          </cell>
+          <cell r="G18"/>
         </row>
         <row r="20">
-          <cell r="G20" t="str">
-            <v>OFF</v>
-          </cell>
+          <cell r="G20"/>
         </row>
         <row r="21">
-          <cell r="G21" t="str">
-            <v>ON</v>
-          </cell>
+          <cell r="G21"/>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1546,114 +1452,121 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="30" customWidth="1"/>
-    <col min="2" max="2" width="11" style="30" customWidth="1"/>
-    <col min="3" max="4" width="14" style="30" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="30" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="30" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="22" customWidth="1"/>
+    <col min="2" max="2" width="11" style="22" customWidth="1"/>
+    <col min="3" max="4" width="14" style="22" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="22" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="55"/>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="49"/>
-      <c r="B3" t="s">
+      <c r="F3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="55"/>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="49"/>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="55"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="I5" s="47"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="55"/>
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="55"/>
+      <c r="B7" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="49"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="49"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="49"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="55"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="14"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
+      <c r="A9" s="55"/>
       <c r="C9"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="20"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="14"/>
+      <c r="I9" s="47"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="A10" s="55"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="38"/>
+      <c r="A11" s="55"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="I11" s="47"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1661,333 +1574,308 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="21" t="s">
+      <c r="F15" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="G15" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="I15" s="21"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="23"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="29"/>
-      <c r="K15" s="29"/>
-    </row>
-    <row r="16" spans="1:11" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="I16" s="31"/>
-      <c r="K16" s="32"/>
-    </row>
-    <row r="17" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27" t="s">
+      <c r="F17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="G17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="17"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="18"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32"/>
+      <c r="B20" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-    </row>
-    <row r="18" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="25"/>
-      <c r="F18" s="31" t="str">
-        <f>IFERROR(INDEX([1]Settings!$A$6:$B$12,MATCH(D18,[1]Settings!$A$6:$A$12,0),2),"")</f>
-        <v/>
-      </c>
-      <c r="G18" s="26"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-    </row>
-    <row r="19" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
-      <c r="B20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="40"/>
-    </row>
-    <row r="21" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="53" t="s">
+      <c r="C20" s="40"/>
+      <c r="D20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="32"/>
+    </row>
+    <row r="22" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="40"/>
-    </row>
-    <row r="22" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="56" t="s">
+      <c r="D22" s="64"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="43" t="s">
+      <c r="D23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="40" t="str">
-        <f t="shared" ref="G22:G29" si="0">IF(AND(F22&lt;&gt;"",B22&lt;&gt;""),F22*B22,"")</f>
-        <v/>
-      </c>
-      <c r="I22" s="39"/>
-    </row>
-    <row r="23" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="56" t="s">
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="43" t="s">
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="56" t="s">
+      <c r="G24" s="32"/>
+    </row>
+    <row r="25" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="43" t="s">
+      <c r="D25" s="64"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="32"/>
+    </row>
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="32"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="40"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="36" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="G27" s="32"/>
+    </row>
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="32"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="40"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="63" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="G34" s="40"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
     </row>
     <row r="37" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B41" s="7"/>

</xml_diff>

<commit_message>
Update settings.py, Addemail alerts and error handling to views.py, Update template folder struct.
</commit_message>
<xml_diff>
--- a/file_manager/rental_order.xlsx
+++ b/file_manager/rental_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikthomas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CB8A8E-3E37-0749-8D20-8D270A033853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F4CBF0-2BA9-EF4E-AD86-10BE998FDE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23820" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>TAGGABOX</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SHIPPED</t>
   </si>
   <si>
     <t>Qty</t>
@@ -185,12 +182,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="@\ \ "/>
-    <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="164" formatCode="@\ \ "/>
+    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -562,15 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -595,7 +585,7 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -610,9 +600,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -637,7 +624,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -654,11 +641,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,16 +674,21 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -726,28 +717,7 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right style="dotted">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top style="dotted">
-          <color rgb="FFFF0000"/>
-        </top>
-        <bottom style="dotted">
-          <color rgb="FFFF0000"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1449,444 +1419,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="22" customWidth="1"/>
-    <col min="2" max="2" width="11" style="22" customWidth="1"/>
-    <col min="3" max="4" width="14" style="22" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="22" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="22" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11" style="19" customWidth="1"/>
+    <col min="3" max="4" width="14" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="19" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="56"/>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="55"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="52"/>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="E3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="55"/>
+      <c r="F3" s="48"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="52"/>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="48"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="52"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="52"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="52"/>
+      <c r="B7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="52"/>
+      <c r="C9"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="12"/>
+      <c r="H9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="H10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="H11" s="43"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="20"/>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="15"/>
+      <c r="F18" s="47"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29"/>
+      <c r="B20" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="61"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="29"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="29"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="25"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="25"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="25"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="25"/>
+      <c r="B33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="25"/>
+      <c r="F33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="55"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="I5" s="47"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="55"/>
-      <c r="I6" s="47"/>
-    </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55"/>
-      <c r="B7" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="14"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="C9"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="14"/>
-      <c r="I9" s="47"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="55"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="I10" s="47"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="55"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="30"/>
-      <c r="I11" s="47"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="23"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-    </row>
-    <row r="18" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="17"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="18"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
-      <c r="B20" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="32"/>
-    </row>
-    <row r="21" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="32"/>
-    </row>
-    <row r="22" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="32"/>
-      <c r="I22" s="31"/>
-    </row>
-    <row r="23" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="32"/>
-    </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="32"/>
-    </row>
-    <row r="25" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="32"/>
-    </row>
-    <row r="26" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="32"/>
-    </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="32"/>
-    </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="1:12" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="32"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="6" t="s">
+      <c r="C34" s="25"/>
+      <c r="D34" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="38" t="s">
+      <c r="E34" s="25"/>
+      <c r="F34" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="32"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-    </row>
-    <row r="37" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="54"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="55"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+    </row>
+    <row r="37" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="51"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="A2:A11"/>
@@ -1902,83 +1842,78 @@
     <mergeCell ref="C29:E29"/>
   </mergeCells>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>(SellerName="")*bSellerName</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="13" priority="18">
       <formula>(SellerAddress="")*bSellerAddress</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>(SellerPhone="")*bSellerPhone</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>(SellerFax="")*bSellerFax</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>(BuyerName="")*bBuyerName</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>(BuyerAddress="")*bBuyerAddress</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>(BuyerCityStateZip="")*bBuyerCity</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>(BuyerPhone="")*bBuyerPhone</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>(BuyerFax="")*bBuyerFax</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$I$13=""</formula>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>$H$13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>(invPONumber="")*bPONumber</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>(invSalesperson="")*bSalesperson</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>(invShippedVia="")*bShippedVia</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>(invTerms="")*bTerms</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>(invFOBIncoterm="")*bFOBIncoterm</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
+  <conditionalFormatting sqref="F18">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$I$13=""</formula>
+      <formula>$H$13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Elastic Beanstalk setup, update handtrucks into models
</commit_message>
<xml_diff>
--- a/file_manager/rental_order.xlsx
+++ b/file_manager/rental_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr updateLinks="always" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikthomas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F4CBF0-2BA9-EF4E-AD86-10BE998FDE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8DF130-F230-4946-95FC-F162D725450E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23820" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
-    <t>TAGGABOX</t>
-  </si>
-  <si>
     <t>Rental Order</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Hand-Truck</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
     <numFmt numFmtId="164" formatCode="@\ \ "/>
     <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,19 +257,27 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF00B050"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <sz val="26"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -553,12 +561,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -592,17 +609,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -613,8 +624,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -641,12 +650,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,37 +659,50 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1044,6 +1060,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>425575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46481A05-525E-0740-9A89-6519FBA89916}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="114300"/>
+          <a:ext cx="1587500" cy="311275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1422,402 +1487,396 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C29" sqref="C29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="11" style="19" customWidth="1"/>
-    <col min="3" max="4" width="14" style="19" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="19" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="17" customWidth="1"/>
+    <col min="2" max="2" width="11" style="17" customWidth="1"/>
+    <col min="3" max="4" width="14" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="17" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B1" s="1"/>
+      <c r="E1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="F1" s="53"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="55"/>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="54"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" t="s">
+      <c r="E3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="51"/>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="41" t="s">
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="51"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="51"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="48"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="H5" s="43"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="H6" s="43"/>
-    </row>
-    <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="51"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
       <c r="C9"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="12"/>
-      <c r="H9" s="43"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="H10" s="43"/>
+      <c r="A10" s="51"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="52"/>
+      <c r="A11" s="51"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="H11" s="43"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13" t="s">
+      <c r="F15" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="H15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="18"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="20"/>
-      <c r="J16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="47"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37" t="s">
+      <c r="D18" s="14"/>
+      <c r="F18" s="36"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="57" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="25"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="60" t="s">
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="25"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="31" t="s">
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="60" t="s">
+    </row>
+    <row r="24" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="31" t="s">
+      <c r="D24" s="60"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="60" t="s">
+    <row r="25" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="25"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="31" t="s">
+      <c r="D25" s="60"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="27"/>
+    </row>
+    <row r="26" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="27"/>
+    </row>
+    <row r="27" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="25"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="31"/>
-    </row>
-    <row r="27" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="25"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
+      <c r="C28" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="61"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:11" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
+    <row r="29" spans="1:11" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="25"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="65"/>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="25"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="25"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="25"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="25"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="21"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="25"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="4" t="s">
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="21"/>
+      <c r="F36" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
+      <c r="B37" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="35"/>
+      <c r="D37" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="34" t="s">
+      <c r="E37" s="35"/>
+      <c r="F37" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-    </row>
-    <row r="37" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="51"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+    </row>
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="34"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1918,5 +1977,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>